<commit_message>
correction API and some cleanup #9
</commit_message>
<xml_diff>
--- a/tests/resources/supercon_corrected.xlsx
+++ b/tests/resources/supercon_corrected.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfoppiano/development/projects/supercon2/resources/sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfoppiano/development/projects/supercon2/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B4DABC-1E89-7047-BB8C-0429977201A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92E97B-B21D-BA4E-8B86-50D9D8546E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="supercon_corrected" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="supercon_corrected" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">supercon_corrected!$A$1:$Y$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">supercon_corrected!$A$1:$Y$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1014,10 +1015,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB64438-5B6C-7940-B998-180F6C5ABE1D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="31"/>
   <cols>

</xml_diff>